<commit_message>
:hammer: updated quick sort testing and PDFs; code formatting
</commit_message>
<xml_diff>
--- a/src/p6/Sorting Graphs.xlsx
+++ b/src/p6/Sorting Graphs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajit Banerjee\Desktop\Algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajit Banerjee\Desktop\Algorithms\algorithm-portfolio-20290-rajitbanerjee\src\p6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47A7739-A23B-4219-9C25-7012B6941A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A39749-8612-4B53-9147-0D6D3BE63BB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="p5" sheetId="1" r:id="rId1"/>
-    <sheet name="p6" sheetId="2" r:id="rId2"/>
+    <sheet name="p4" sheetId="3" r:id="rId1"/>
+    <sheet name="p5" sheetId="1" r:id="rId2"/>
+    <sheet name="p6" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Time (in nanoseconds)</t>
   </si>
@@ -37,9 +38,6 @@
     <t>Merge Sort</t>
   </si>
   <si>
-    <t>Fast Merge Sort</t>
-  </si>
-  <si>
     <t>Array Size</t>
   </si>
   <si>
@@ -47,6 +45,15 @@
   </si>
   <si>
     <t>Enhanced Quick Sort</t>
+  </si>
+  <si>
+    <t>Selection Sort</t>
+  </si>
+  <si>
+    <t>Bogo Sort</t>
+  </si>
+  <si>
+    <t>Enhanced Merge Sort</t>
   </si>
 </sst>
 </file>
@@ -90,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -106,6 +113,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -159,11 +169,708 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> taken vs Number of elements</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'p4'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'p4'!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'p4'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>85400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>651400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17440000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>185364400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C97A-43F1-A972-E733251CF3B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'p4'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'p4'!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'p4'!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>129800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>430300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17495200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>249887400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C97A-43F1-A972-E733251CF3B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1682794304"/>
+        <c:axId val="1556592320"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Bogo Sort</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'p4'!$A$3:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'p4'!$D$3:$D$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>34550400</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1442261400</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="1"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-C97A-43F1-A972-E733251CF3B4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1682794304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of elements in array being sorted</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1556592320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1556592320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time taken (nanoseconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1682794304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Sorting</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Time Compasrion (Insertion, Merge, Fast Merge)</a:t>
+              <a:t> Time Comparison </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>(Insertion, Merge, Enhanced Merge)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -249,10 +956,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -265,9 +972,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -279,25 +983,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>38800</c:v>
+                  <c:v>42200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10500</c:v>
+                  <c:v>54400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65800</c:v>
+                  <c:v>115200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>565200</c:v>
+                  <c:v>1425500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1890600</c:v>
+                  <c:v>13609100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18997600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37792600</c:v>
+                  <c:v>182815900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,10 +1047,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -362,9 +1063,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,25 +1074,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>85300</c:v>
+                  <c:v>25500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12300</c:v>
+                  <c:v>17800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113400</c:v>
+                  <c:v>21000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10633400</c:v>
+                  <c:v>1281600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19370000</c:v>
+                  <c:v>137560300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>955170700</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3859741400</c:v>
+                  <c:v>18319241800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,7 +1110,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fast Merge Sort</c:v>
+                  <c:v>Enhanced Merge Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -451,10 +1146,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -467,9 +1162,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -481,25 +1173,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19800</c:v>
+                  <c:v>100100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3800</c:v>
+                  <c:v>13900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14700</c:v>
+                  <c:v>112100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88300</c:v>
+                  <c:v>758100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>851900</c:v>
+                  <c:v>3868800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10994500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27065700</c:v>
+                  <c:v>95411100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -526,6 +1215,7 @@
         <c:axId val="997426495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -643,6 +1333,7 @@
         <c:axId val="868922559"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -685,7 +1376,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> taken (in nanoseconds)</a:t>
+                  <a:t> taken (nanoseconds)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -844,7 +1535,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -883,7 +1574,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Sort vs Fast Merge Sort</a:t>
+              <a:t> Sort vs Enhanced Merge Sort</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -969,10 +1660,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -985,9 +1676,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,25 +1687,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>38800</c:v>
+                  <c:v>42200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10500</c:v>
+                  <c:v>54400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65800</c:v>
+                  <c:v>115200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>565200</c:v>
+                  <c:v>1425500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1890600</c:v>
+                  <c:v>13609100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18997600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37792600</c:v>
+                  <c:v>182815900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,7 +1723,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fast Merge Sort</c:v>
+                  <c:v>Enhanced Merge Sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1074,10 +1759,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -1090,9 +1775,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1104,25 +1786,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19800</c:v>
+                  <c:v>100100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3800</c:v>
+                  <c:v>13900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14700</c:v>
+                  <c:v>112100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88300</c:v>
+                  <c:v>758100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>851900</c:v>
+                  <c:v>3868800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10994500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27065700</c:v>
+                  <c:v>95411100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1149,6 +1828,7 @@
         <c:axId val="1005778479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1227,7 +1907,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1271,6 +1951,7 @@
         <c:axId val="868923807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1313,7 +1994,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>e taken (in nanosecods)</a:t>
+                  <a:t>e taken (nanosecods)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1348,7 +2029,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1471,7 +2152,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1596,10 +2277,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -1612,9 +2293,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,25 +2304,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>123900</c:v>
+                  <c:v>127000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25900</c:v>
+                  <c:v>41000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>139100</c:v>
+                  <c:v>275700</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1148400</c:v>
+                  <c:v>1766800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4371400</c:v>
+                  <c:v>7413700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24895800</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37046500</c:v>
+                  <c:v>165088600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,10 +2376,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -1717,9 +2392,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1731,25 +2403,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>23000</c:v>
+                  <c:v>25200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6600</c:v>
+                  <c:v>9400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38300</c:v>
+                  <c:v>46200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>322700</c:v>
+                  <c:v>642300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1015200</c:v>
+                  <c:v>2667500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9194800</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16560900</c:v>
+                  <c:v>91046700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1806,10 +2475,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -1822,9 +2491,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1836,25 +2502,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>20000</c:v>
+                  <c:v>182800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5300</c:v>
+                  <c:v>11400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17700</c:v>
+                  <c:v>51200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>122000</c:v>
+                  <c:v>558400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>918900</c:v>
+                  <c:v>4740800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6880600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14275600</c:v>
+                  <c:v>38632900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,6 +2544,7 @@
         <c:axId val="997426495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1998,6 +2662,7 @@
         <c:axId val="868922559"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2040,7 +2705,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> taken (in nanoseconds)</a:t>
+                  <a:t> taken (nanoseconds)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2319,6 +2984,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3867,20 +4572,577 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>253999</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66487</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>388470</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B5FAE5-30E7-4F2E-8284-C02DE9606151}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>261471</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>51546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>395942</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>141941</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3944,7 +5206,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4249,11 +5511,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429FB3B0-3F0C-4B4A-B6DF-A764BE244366}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>85400</v>
+      </c>
+      <c r="C3" s="1">
+        <v>129800</v>
+      </c>
+      <c r="D3" s="1">
+        <v>34550400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>16800</v>
+      </c>
+      <c r="C4" s="1">
+        <v>17900</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1442261400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>100</v>
+      </c>
+      <c r="B5" s="1">
+        <v>651400</v>
+      </c>
+      <c r="C5" s="1">
+        <v>430300</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>17440000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>17495200</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>185364400</v>
+      </c>
+      <c r="C7" s="1">
+        <v>249887400</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4261,19 +5635,19 @@
     <col min="1" max="1" width="10.90625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
@@ -4284,35 +5658,35 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>85300</v>
+        <v>25500</v>
       </c>
       <c r="C3" s="1">
-        <v>38800</v>
+        <v>42200</v>
       </c>
       <c r="D3" s="1">
-        <v>19800</v>
+        <v>100100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>12300</v>
+        <v>17800</v>
       </c>
       <c r="C4" s="1">
-        <v>10500</v>
+        <v>54400</v>
       </c>
       <c r="D4" s="1">
-        <v>3800</v>
+        <v>13900</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -4320,13 +5694,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="1">
-        <v>113400</v>
+        <v>21000</v>
       </c>
       <c r="C5" s="1">
-        <v>65800</v>
+        <v>115200</v>
       </c>
       <c r="D5" s="1">
-        <v>14700</v>
+        <v>112100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -4334,13 +5708,13 @@
         <v>1000</v>
       </c>
       <c r="B6" s="1">
-        <v>10633400</v>
+        <v>1281600</v>
       </c>
       <c r="C6" s="1">
-        <v>565200</v>
+        <v>1425500</v>
       </c>
       <c r="D6" s="1">
-        <v>88300</v>
+        <v>758100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -4348,13 +5722,13 @@
         <v>10000</v>
       </c>
       <c r="B7" s="1">
-        <v>19370000</v>
+        <v>137560300</v>
       </c>
       <c r="C7" s="1">
-        <v>1890600</v>
+        <v>13609100</v>
       </c>
       <c r="D7" s="1">
-        <v>851900</v>
+        <v>3868800</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -4362,27 +5736,13 @@
         <v>100000</v>
       </c>
       <c r="B8" s="1">
-        <v>955170700</v>
+        <v>18319241800</v>
       </c>
       <c r="C8" s="1">
-        <v>18997600</v>
+        <v>182815900</v>
       </c>
       <c r="D8" s="1">
-        <v>10994500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>200000</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3859741400</v>
-      </c>
-      <c r="C9" s="1">
-        <v>37792600</v>
-      </c>
-      <c r="D9" s="1">
-        <v>27065700</v>
+        <v>95411100</v>
       </c>
     </row>
   </sheetData>
@@ -4396,12 +5756,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF74F750-086E-4DCB-81A5-6F194E46E18D}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4414,13 +5774,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
@@ -4428,38 +5788,38 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>123900</v>
+        <v>127000</v>
       </c>
       <c r="C3" s="1">
-        <v>23000</v>
+        <v>25200</v>
       </c>
       <c r="D3" s="1">
-        <v>20000</v>
+        <v>182800</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>25900</v>
+        <v>41000</v>
       </c>
       <c r="C4" s="1">
-        <v>6600</v>
+        <v>9400</v>
       </c>
       <c r="D4" s="1">
-        <v>5300</v>
+        <v>11400</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -4467,13 +5827,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="1">
-        <v>139100</v>
+        <v>275700</v>
       </c>
       <c r="C5" s="1">
-        <v>38300</v>
+        <v>46200</v>
       </c>
       <c r="D5" s="1">
-        <v>17700</v>
+        <v>51200</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -4481,13 +5841,13 @@
         <v>1000</v>
       </c>
       <c r="B6" s="1">
-        <v>1148400</v>
+        <v>1766800</v>
       </c>
       <c r="C6" s="1">
-        <v>322700</v>
+        <v>642300</v>
       </c>
       <c r="D6" s="1">
-        <v>122000</v>
+        <v>558400</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -4495,13 +5855,13 @@
         <v>10000</v>
       </c>
       <c r="B7" s="1">
-        <v>4371400</v>
+        <v>7413700</v>
       </c>
       <c r="C7" s="1">
-        <v>1015200</v>
+        <v>2667500</v>
       </c>
       <c r="D7" s="1">
-        <v>918900</v>
+        <v>4740800</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -4509,28 +5869,20 @@
         <v>100000</v>
       </c>
       <c r="B8" s="1">
-        <v>24895800</v>
+        <v>165088600</v>
       </c>
       <c r="C8" s="1">
-        <v>9194800</v>
+        <v>91046700</v>
       </c>
       <c r="D8" s="1">
-        <v>6880600</v>
+        <v>38632900</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>200000</v>
-      </c>
-      <c r="B9" s="1">
-        <v>37046500</v>
-      </c>
-      <c r="C9" s="1">
-        <v>16560900</v>
-      </c>
-      <c r="D9" s="1">
-        <v>14275600</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C16" s="3"/>

</xml_diff>

<commit_message>
:books: add some graphs and update README to summarise documentation files
</commit_message>
<xml_diff>
--- a/src/p6/Sorting Graphs.xlsx
+++ b/src/p6/Sorting Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajit Banerjee\Desktop\Algorithms\algorithm-portfolio-20290-rajitbanerjee\src\p6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A39749-8612-4B53-9147-0D6D3BE63BB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E5F613-D83F-4260-AF17-854762A39BA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="p4" sheetId="3" r:id="rId1"/>
@@ -5514,8 +5514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429FB3B0-3F0C-4B4A-B6DF-A764BE244366}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5626,7 +5626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>

</xml_diff>